<commit_message>
Fix spreadsheet column address parsing
</commit_message>
<xml_diff>
--- a/tests/empty_cells.xlsx
+++ b/tests/empty_cells.xlsx
@@ -10,6 +10,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Big col nums" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">Cell B2</t>
   </si>
@@ -33,6 +34,12 @@
   </si>
   <si>
     <t xml:space="preserve">Cell F6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cell Z1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cell AA2</t>
   </si>
 </sst>
 </file>
@@ -47,6 +54,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -106,8 +114,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -134,15 +146,15 @@
       <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
     </row>
@@ -168,22 +180,56 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regularna"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regularna"&amp;12Strona &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="Z1:AA2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Z1" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA2" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regularna"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regularna"&amp;12Strona &amp;P</oddFooter>

</xml_diff>